<commit_message>
new directory structure in code with +
</commit_message>
<xml_diff>
--- a/SCOPE_v1.70/input_data.xlsx
+++ b/SCOPE_v1.70/input_data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\tol\models\forward\SCOPE\SCOPE_v1.70\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects Python\SCOPE\SCOPE_v1.70\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12240" windowHeight="5568" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12240" windowHeight="5568" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="5" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="filenames" sheetId="3" r:id="rId3"/>
     <sheet name="inputdata" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -1271,7 +1271,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1696,6 +1696,8 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1705,8 +1707,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2306,20 +2306,20 @@
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56" s="49" t="s">
+      <c r="A56" s="51" t="s">
         <v>128</v>
       </c>
-      <c r="B56" s="49" t="s">
+      <c r="B56" s="51" t="s">
         <v>108</v>
       </c>
-      <c r="C56" s="49" t="s">
+      <c r="C56" s="51" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="50"/>
-      <c r="B57" s="50"/>
-      <c r="C57" s="50"/>
+      <c r="A57" s="52"/>
+      <c r="B57" s="52"/>
+      <c r="C57" s="52"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="11" t="s">
@@ -2395,13 +2395,13 @@
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" s="15"/>
       <c r="B68" s="16"/>
-      <c r="C68" s="51" t="s">
+      <c r="C68" s="53" t="s">
         <v>235</v>
       </c>
-      <c r="D68" s="52"/>
-      <c r="E68" s="52"/>
-      <c r="F68" s="52"/>
-      <c r="G68" s="53"/>
+      <c r="D68" s="54"/>
+      <c r="E68" s="54"/>
+      <c r="F68" s="54"/>
+      <c r="G68" s="55"/>
       <c r="H68" s="17"/>
       <c r="I68" s="17"/>
       <c r="J68" s="18"/>
@@ -3004,7 +3004,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="93" spans="1:10" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A93" s="39" t="s">
         <v>303</v>
       </c>
@@ -3101,8 +3101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3313,7 +3313,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C22" t="s">
         <v>51</v>
@@ -3344,7 +3344,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
@@ -3526,7 +3526,7 @@
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="55" t="s">
+      <c r="A32" s="50" t="s">
         <v>345</v>
       </c>
     </row>
@@ -3536,7 +3536,7 @@
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" s="54"/>
+      <c r="A34" s="49"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>

</xml_diff>